<commit_message>
data collection complete, excel created
</commit_message>
<xml_diff>
--- a/results/Data.xlsx
+++ b/results/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\PycharmProjects\project-athena\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B12D104-B5B3-4DA4-83EC-AFEC7976DF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FB9F6C-E18C-4A33-B59A-24F56770B901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{020305A6-F778-4984-84A1-ABAB69C2609E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="155">
   <si>
     <t>UM</t>
   </si>
@@ -494,6 +494,12 @@
   </si>
   <si>
     <t>[7, 19, 24, 53, 56]</t>
+  </si>
+  <si>
+    <t>in Min</t>
+  </si>
+  <si>
+    <t>In hour</t>
   </si>
 </sst>
 </file>
@@ -881,15 +887,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24AF8C9C-7B73-4240-9BB9-D32E4C28AAB4}">
-  <dimension ref="A1:BE45"/>
+  <dimension ref="A1:BD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="AU23" sqref="AU23"/>
+    <sheetView tabSelected="1" topLeftCell="AJ24" zoomScale="102" workbookViewId="0">
+      <selection activeCell="BB43" sqref="BB43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54">
@@ -2349,7 +2356,7 @@
         <v>3.03336703741152E-3</v>
       </c>
       <c r="BB9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9:BA9)</f>
         <v>2.1031344792719887E-2</v>
       </c>
     </row>
@@ -3508,7 +3515,7 @@
         <v>3.9089989888776502E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:55">
+    <row r="17" spans="1:56">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3673,7 +3680,7 @@
         <v>3.1466127401415515E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:55">
+    <row r="18" spans="1:56">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -3838,7 +3845,7 @@
         <v>2.4266936299292184E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:55">
+    <row r="19" spans="1:56">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -4003,7 +4010,7 @@
         <v>4.4893832153690555E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:55">
+    <row r="20" spans="1:56">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -4168,7 +4175,7 @@
         <v>4.3013144590495378E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:55">
+    <row r="21" spans="1:56">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4333,7 +4340,7 @@
         <v>2.7017189079878635E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:55">
+    <row r="22" spans="1:56">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -4542,7 +4549,7 @@
         <v>7.5609482080665064E-2</v>
       </c>
       <c r="BA22">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(BA4:BA21)</f>
         <v>1.2526682395236473E-2</v>
       </c>
       <c r="BB22">
@@ -4550,7 +4557,7 @@
         <v>3.9350634760139273E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:55">
+    <row r="23" spans="1:56">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -4607,7 +4614,7 @@
       <c r="BB23" s="5"/>
       <c r="BC23" s="5"/>
     </row>
-    <row r="24" spans="1:55">
+    <row r="24" spans="1:56">
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -4767,8 +4774,14 @@
       <c r="BB24" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="BC24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="BD24" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="25" spans="1:55">
+    <row r="25" spans="1:56">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -4927,11 +4940,11 @@
         <v>592.77465332031147</v>
       </c>
       <c r="BC25">
-        <f t="shared" ref="BC25:BC42" si="5">BB25/60</f>
+        <f>BB25/60</f>
         <v>9.8795775553385248</v>
       </c>
     </row>
-    <row r="26" spans="1:55">
+    <row r="26" spans="1:56">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -5086,15 +5099,15 @@
         <v>101.201553106307</v>
       </c>
       <c r="BB26">
-        <f t="shared" ref="BB26:BB45" si="6">AVERAGE(D26:BA26)</f>
+        <f t="shared" ref="BB26:BB45" si="5">AVERAGE(D26:BA26)</f>
         <v>580.37237195491707</v>
       </c>
       <c r="BC26">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="BC25:BC42" si="6">BB26/60</f>
         <v>9.6728728659152843</v>
       </c>
     </row>
-    <row r="27" spans="1:55">
+    <row r="27" spans="1:56">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -5249,15 +5262,15 @@
         <v>101.453325510025</v>
       </c>
       <c r="BB27">
+        <f t="shared" si="5"/>
+        <v>580.13917757034176</v>
+      </c>
+      <c r="BC27">
         <f t="shared" si="6"/>
-        <v>580.13917757034176</v>
-      </c>
-      <c r="BC27">
-        <f t="shared" si="5"/>
         <v>9.6689862928390298</v>
       </c>
     </row>
-    <row r="28" spans="1:55">
+    <row r="28" spans="1:56">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -5412,15 +5425,15 @@
         <v>101.782147884368</v>
       </c>
       <c r="BB28">
+        <f t="shared" si="5"/>
+        <v>581.67827337264862</v>
+      </c>
+      <c r="BC28">
         <f t="shared" si="6"/>
-        <v>581.67827337264862</v>
-      </c>
-      <c r="BC28">
-        <f t="shared" si="5"/>
         <v>9.6946378895441434</v>
       </c>
     </row>
-    <row r="29" spans="1:55">
+    <row r="29" spans="1:56">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -5575,15 +5588,15 @@
         <v>101.92251443862899</v>
       </c>
       <c r="BB29">
+        <f t="shared" si="5"/>
+        <v>575.84795341968425</v>
+      </c>
+      <c r="BC29">
         <f t="shared" si="6"/>
-        <v>575.84795341968425</v>
-      </c>
-      <c r="BC29">
-        <f t="shared" si="5"/>
         <v>9.5974658903280705</v>
       </c>
     </row>
-    <row r="30" spans="1:55">
+    <row r="30" spans="1:56">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -5738,15 +5751,15 @@
         <v>100.490602254867</v>
       </c>
       <c r="BB30">
+        <f t="shared" si="5"/>
+        <v>1154.432002663611</v>
+      </c>
+      <c r="BC30">
         <f t="shared" si="6"/>
-        <v>1154.432002663611</v>
-      </c>
-      <c r="BC30">
-        <f t="shared" si="5"/>
         <v>19.240533377726852</v>
       </c>
     </row>
-    <row r="31" spans="1:55">
+    <row r="31" spans="1:56">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -5901,15 +5914,15 @@
         <v>100.331343889236</v>
       </c>
       <c r="BB31">
+        <f t="shared" si="5"/>
+        <v>577.90161647796481</v>
+      </c>
+      <c r="BC31">
         <f t="shared" si="6"/>
-        <v>577.90161647796481</v>
-      </c>
-      <c r="BC31">
-        <f t="shared" si="5"/>
         <v>9.6316936079660795</v>
       </c>
     </row>
-    <row r="32" spans="1:55">
+    <row r="32" spans="1:56">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -6064,15 +6077,15 @@
         <v>100.41890835762</v>
       </c>
       <c r="BB32">
+        <f t="shared" si="5"/>
+        <v>582.58829443454647</v>
+      </c>
+      <c r="BC32">
         <f t="shared" si="6"/>
-        <v>582.58829443454647</v>
-      </c>
-      <c r="BC32">
-        <f t="shared" si="5"/>
         <v>9.7098049072424413</v>
       </c>
     </row>
-    <row r="33" spans="1:57">
+    <row r="33" spans="1:56">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -6227,15 +6240,15 @@
         <v>100.895277738571</v>
       </c>
       <c r="BB33">
+        <f t="shared" si="5"/>
+        <v>582.61190745830402</v>
+      </c>
+      <c r="BC33">
         <f t="shared" si="6"/>
-        <v>582.61190745830402</v>
-      </c>
-      <c r="BC33">
-        <f t="shared" si="5"/>
         <v>9.7101984576384002</v>
       </c>
     </row>
-    <row r="34" spans="1:57">
+    <row r="34" spans="1:56">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -6390,15 +6403,15 @@
         <v>100.517026901245</v>
       </c>
       <c r="BB34">
+        <f t="shared" si="5"/>
+        <v>578.93994749545948</v>
+      </c>
+      <c r="BC34">
         <f t="shared" si="6"/>
-        <v>578.93994749545948</v>
-      </c>
-      <c r="BC34">
-        <f t="shared" si="5"/>
         <v>9.648999124924325</v>
       </c>
     </row>
-    <row r="35" spans="1:57">
+    <row r="35" spans="1:56">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -6553,15 +6566,15 @@
         <v>99.731331110000596</v>
       </c>
       <c r="BB35">
+        <f t="shared" si="5"/>
+        <v>577.81227035522329</v>
+      </c>
+      <c r="BC35">
         <f t="shared" si="6"/>
-        <v>577.81227035522329</v>
-      </c>
-      <c r="BC35">
-        <f t="shared" si="5"/>
         <v>9.6302045059203873</v>
       </c>
     </row>
-    <row r="36" spans="1:57">
+    <row r="36" spans="1:56">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -6716,15 +6729,15 @@
         <v>99.275678634643498</v>
       </c>
       <c r="BB36">
+        <f t="shared" si="5"/>
+        <v>578.50750622749217</v>
+      </c>
+      <c r="BC36">
         <f t="shared" si="6"/>
-        <v>578.50750622749217</v>
-      </c>
-      <c r="BC36">
-        <f t="shared" si="5"/>
         <v>9.6417917704582035</v>
       </c>
     </row>
-    <row r="37" spans="1:57">
+    <row r="37" spans="1:56">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -6879,15 +6892,15 @@
         <v>99.159111261367798</v>
       </c>
       <c r="BB37">
+        <f t="shared" si="5"/>
+        <v>576.76901179313541</v>
+      </c>
+      <c r="BC37">
         <f t="shared" si="6"/>
-        <v>576.76901179313541</v>
-      </c>
-      <c r="BC37">
-        <f t="shared" si="5"/>
         <v>9.6128168632189226</v>
       </c>
     </row>
-    <row r="38" spans="1:57">
+    <row r="38" spans="1:56">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -7042,15 +7055,15 @@
         <v>101.620849847793</v>
       </c>
       <c r="BB38">
+        <f t="shared" si="5"/>
+        <v>579.34019112586896</v>
+      </c>
+      <c r="BC38">
         <f t="shared" si="6"/>
-        <v>579.34019112586896</v>
-      </c>
-      <c r="BC38">
-        <f t="shared" si="5"/>
         <v>9.6556698520978159</v>
       </c>
     </row>
-    <row r="39" spans="1:57">
+    <row r="39" spans="1:56">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -7205,15 +7218,15 @@
         <v>101.66282105445801</v>
       </c>
       <c r="BB39">
+        <f t="shared" si="5"/>
+        <v>580.02498432636128</v>
+      </c>
+      <c r="BC39">
         <f t="shared" si="6"/>
-        <v>580.02498432636128</v>
-      </c>
-      <c r="BC39">
-        <f t="shared" si="5"/>
         <v>9.6670830721060206</v>
       </c>
     </row>
-    <row r="40" spans="1:57">
+    <row r="40" spans="1:56">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -7368,15 +7381,15 @@
         <v>101.486025333404</v>
       </c>
       <c r="BB40">
+        <f t="shared" si="5"/>
+        <v>580.81711812496087</v>
+      </c>
+      <c r="BC40">
         <f t="shared" si="6"/>
-        <v>580.81711812496087</v>
-      </c>
-      <c r="BC40">
-        <f t="shared" si="5"/>
         <v>9.680285302082682</v>
       </c>
     </row>
-    <row r="41" spans="1:57">
+    <row r="41" spans="1:56">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -7531,15 +7544,15 @@
         <v>100.70778465270899</v>
       </c>
       <c r="BB41">
+        <f t="shared" si="5"/>
+        <v>578.51235760688655</v>
+      </c>
+      <c r="BC41">
         <f t="shared" si="6"/>
-        <v>578.51235760688655</v>
-      </c>
-      <c r="BC41">
-        <f t="shared" si="5"/>
         <v>9.6418726267814421</v>
       </c>
     </row>
-    <row r="42" spans="1:57">
+    <row r="42" spans="1:56">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -7694,15 +7707,15 @@
         <v>101.238223791122</v>
       </c>
       <c r="BB42">
+        <f t="shared" si="5"/>
+        <v>580.81696214675753</v>
+      </c>
+      <c r="BC42">
         <f t="shared" si="6"/>
-        <v>580.81696214675753</v>
-      </c>
-      <c r="BC42">
-        <f t="shared" si="5"/>
         <v>9.6802827024459592</v>
       </c>
     </row>
-    <row r="43" spans="1:57">
+    <row r="43" spans="1:56">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -7869,12 +7882,8 @@
         <f>BC43/60</f>
         <v>153.05399089150939</v>
       </c>
-      <c r="BE43">
-        <f>BD43/5</f>
-        <v>30.610798178301877</v>
-      </c>
     </row>
-    <row r="44" spans="1:57">
+    <row r="44" spans="1:56">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -8079,11 +8088,11 @@
         <v>103.03762609428789</v>
       </c>
       <c r="BB44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>612.21592221524861</v>
       </c>
     </row>
-    <row r="45" spans="1:57">
+    <row r="45" spans="1:56">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -8288,7 +8297,7 @@
         <v>1.7172937682381315</v>
       </c>
       <c r="BB45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10.203598703587474</v>
       </c>
     </row>

</xml_diff>